<commit_message>
Reorganize file structure and start to play around with excel library
</commit_message>
<xml_diff>
--- a/excelsheets/test.xlsx
+++ b/excelsheets/test.xlsx
@@ -5,14 +5,14 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TimmyC/Desktop/astral-grow-shopify-api/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TimmyC/Desktop/astral-grow-shopify-api/excelsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="test" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -353,7 +353,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Can now create a store object with products linked to it
</commit_message>
<xml_diff>
--- a/excelsheets/test.xlsx
+++ b/excelsheets/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="360" yWindow="7360" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -36,13 +33,39 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>Product ID</t>
+  </si>
+  <si>
+    <t>Variant ID</t>
+  </si>
+  <si>
+    <t>20465563205743</t>
+  </si>
+  <si>
+    <t>2182140952687</t>
+  </si>
+  <si>
+    <t>Test Light</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,13 +91,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -350,27 +378,201 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="1" customWidth="1"/>
+    <col min="3" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>